<commit_message>
Modification test de index, finalisation de model et création de objects.xlsx
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projets\athome\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\athome\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="98">
   <si>
     <t>Modèles</t>
   </si>
@@ -234,13 +234,171 @@
     <t>cartModel.php</t>
   </si>
   <si>
+    <t>Créer un nouveau panier</t>
+  </si>
+  <si>
+    <t>Modifier information</t>
+  </si>
+  <si>
+    <t>user, tag, info</t>
+  </si>
+  <si>
+    <t>Update une ligne selon la requete</t>
+  </si>
+  <si>
+    <t>Executer une query</t>
+  </si>
+  <si>
+    <t>query SQL (string)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute directement la query sans la composer </t>
+  </si>
+  <si>
+    <t>Mettre à jour SQL</t>
+  </si>
+  <si>
+    <r>
+      <t>Modifie l'objet user dans SESSION si connecté
+sinon Modifie l'objet user
+Utilise "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mettre à jour SQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>utilise "Créer un nouveau panier"
+Créer la requete et utilise "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>insérer SQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" &amp; 
+Utilise "Connexion utilisateur"</t>
+    </r>
+  </si>
+  <si>
+    <t>id user</t>
+  </si>
+  <si>
+    <r>
+      <t>Utilise "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>insérer SQ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L" pour créer le nouveau panier dans SQL
+Créé et retourne l'objet</t>
+    </r>
+  </si>
+  <si>
+    <t>cartRelationModel</t>
+  </si>
+  <si>
+    <t>Gère les relation entre
+les pieces et le panier
+(quantitée)</t>
+  </si>
+  <si>
+    <t>cartRelationModel.php</t>
+  </si>
+  <si>
+    <t>Obtenir par cart</t>
+  </si>
+  <si>
+    <t>id cart</t>
+  </si>
+  <si>
+    <t>Insérer nouvelle cartRelation</t>
+  </si>
+  <si>
+    <t>id cart, quantité</t>
+  </si>
+  <si>
+    <r>
+      <t>Créer une requete avec "WHERE"
+Utilise "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Obtenir résultat SQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"
+Créer les objets cartrelation
+Retourner un tableaux</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>Créer la requete et utilise "</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="8" tint="-0.249977111117893"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -255,18 +413,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>" &amp; 
-utilise "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Créer un nouveau panier</t>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Gère les différents
+type de piece</t>
+  </si>
+  <si>
+    <t>pieceTypeModel.php</t>
+  </si>
+  <si>
+    <t>Créer un nouveau type</t>
+  </si>
+  <si>
+    <t>label, img_present…</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> utilise "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>insérer SQL</t>
     </r>
     <r>
       <rPr>
@@ -280,7 +455,152 @@
     </r>
   </si>
   <si>
-    <t>Créer un nouveau panier</t>
+    <t>Supprimer un type</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Supprimer SQL</t>
+  </si>
+  <si>
+    <t>Supprime une entrée SQL</t>
+  </si>
+  <si>
+    <t>Mettre à jour le type</t>
+  </si>
+  <si>
+    <t>objet type</t>
+  </si>
+  <si>
+    <r>
+      <t>Utilise "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mettre à jour SQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Obtenir type</t>
+  </si>
+  <si>
+    <t>label, id</t>
+  </si>
+  <si>
+    <r>
+      <t>Utilise "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Obtenir résultat SQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Gère les différents
+style de piece</t>
+  </si>
+  <si>
+    <t>pieceStyleModel.php</t>
+  </si>
+  <si>
+    <t>Créer un nouveau style</t>
+  </si>
+  <si>
+    <t>Supprimer un style</t>
+  </si>
+  <si>
+    <t>Mettre à jour le style</t>
+  </si>
+  <si>
+    <t>objet style</t>
+  </si>
+  <si>
+    <t>Obtenir style</t>
+  </si>
+  <si>
+    <t>commentModel</t>
+  </si>
+  <si>
+    <t>pieceStyleModel</t>
+  </si>
+  <si>
+    <t>pieceTypeModel</t>
+  </si>
+  <si>
+    <t>Gère les commentaires</t>
+  </si>
+  <si>
+    <t>commentModel.php</t>
+  </si>
+  <si>
+    <t>Supprimer un commentaire</t>
+  </si>
+  <si>
+    <t>Obtenir commentaire</t>
+  </si>
+  <si>
+    <t>Créer un nouveau commentaire</t>
+  </si>
+  <si>
+    <t>text, score…</t>
+  </si>
+  <si>
+    <r>
+      <t>Utilise "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Supprimer SQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -311,13 +631,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
+      <color theme="8" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,6 +668,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAB7EF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F8AE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -361,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -376,12 +720,34 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE8F8AE"/>
+      <color rgb="FFEAB7EF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -656,18 +1022,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" customWidth="1"/>
     <col min="6" max="6" width="57.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -770,7 +1136,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -781,7 +1147,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -824,13 +1190,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
@@ -878,15 +1250,19 @@
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
@@ -896,169 +1272,401 @@
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="36" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1" t="s">
+      <c r="E56" s="1"/>
+      <c r="F56" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cart.php + html css cart_item
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="106">
   <si>
     <t>Modèles</t>
   </si>
@@ -237,12 +237,6 @@
     <t>Créer un nouveau panier</t>
   </si>
   <si>
-    <t>Modifier information</t>
-  </si>
-  <si>
-    <t>user, tag, info</t>
-  </si>
-  <si>
     <t>Update une ligne selon la requete</t>
   </si>
   <si>
@@ -256,33 +250,6 @@
   </si>
   <si>
     <t>Mettre à jour SQL</t>
-  </si>
-  <si>
-    <r>
-      <t>Modifie l'objet user dans SESSION si connecté
-sinon Modifie l'objet user
-Utilise "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mettre à jour SQL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
   </si>
   <si>
     <r>
@@ -601,6 +568,62 @@
       </rPr>
       <t>"</t>
     </r>
+  </si>
+  <si>
+    <t>Déconnexion utilisateur</t>
+  </si>
+  <si>
+    <t>Vide _SESSION[user] et rafraichi</t>
+  </si>
+  <si>
+    <t>Actualiser l'utilisateur</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <r>
+      <t>Modifie l'objet user
+Utilise "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mettre à jour SQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Actualiser le meuble</t>
+  </si>
+  <si>
+    <t>piece</t>
+  </si>
+  <si>
+    <t>Actualiser le style</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>Actualiser le cart relation</t>
+  </si>
+  <si>
+    <t>cart relation</t>
   </si>
 </sst>
 </file>
@@ -1024,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:F58"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,9 +1127,15 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -1147,7 +1176,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1190,18 +1219,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1216,9 +1245,13 @@
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
@@ -1258,10 +1291,10 @@
         <v>45</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1274,13 +1307,13 @@
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -1291,13 +1324,13 @@
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E25" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1305,22 +1338,28 @@
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
+      <c r="D27" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -1340,13 +1379,13 @@
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
@@ -1357,13 +1396,13 @@
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1371,13 +1410,13 @@
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1385,13 +1424,13 @@
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1399,32 +1438,38 @@
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
+      <c r="D36" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
@@ -1435,13 +1480,13 @@
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1449,13 +1494,13 @@
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1463,13 +1508,13 @@
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1477,32 +1522,38 @@
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
+      <c r="D43" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="15" t="s">
-        <v>91</v>
-      </c>
       <c r="C45" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
@@ -1513,13 +1564,13 @@
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1527,13 +1578,13 @@
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
       <c r="D47" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1541,13 +1592,13 @@
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
       <c r="D48" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1597,13 +1648,13 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1611,13 +1662,13 @@
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1625,13 +1676,13 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
save 05/02 / création models et objects
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\athome\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projet\athome\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -183,11 +183,6 @@
     <t>mail, password</t>
   </si>
   <si>
-    <t>Utilise "Obtenir résultat SQL" en utilisant une requete avec "WHERE"
-Si aucune ligne n'est retourné, alors le login est faux
-Si une ligne est retourné alors contruire l'objet CurrentUser et l'inserer dans _SESSION</t>
-  </si>
-  <si>
     <t>Obtenir l'utilisateur courant</t>
   </si>
   <si>
@@ -624,6 +619,33 @@
   </si>
   <si>
     <t>cart relation</t>
+  </si>
+  <si>
+    <r>
+      <t>Utilise "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Obtenir résultat SQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" en utilisant une requete avec "WHERE"
+Si aucune ligne n'est retourné, alors le login est faux
+Si une ligne est retourné alors contruire l'objet CurrentUser et l'inserer dans _SESSION</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1047,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,13 +1150,13 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1176,7 +1198,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1184,13 +1206,13 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1204,7 +1226,7 @@
         <v>35</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1212,11 +1234,11 @@
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1224,13 +1246,13 @@
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1246,11 +1268,11 @@
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1271,13 +1293,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -1288,13 +1310,13 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1307,13 +1329,13 @@
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -1324,13 +1346,13 @@
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>58</v>
-      </c>
       <c r="F25" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1338,13 +1360,13 @@
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>60</v>
-      </c>
       <c r="F26" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1352,13 +1374,13 @@
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>105</v>
-      </c>
       <c r="F27" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1379,13 +1401,13 @@
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B31" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>64</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
@@ -1396,13 +1418,13 @@
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="F32" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1410,13 +1432,13 @@
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="11" t="s">
-        <v>69</v>
-      </c>
       <c r="F33" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1424,13 +1446,13 @@
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="F34" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1438,13 +1460,13 @@
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="F35" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1452,24 +1474,24 @@
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E36" s="11" t="s">
-        <v>101</v>
-      </c>
       <c r="F36" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B38" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>78</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>79</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
@@ -1480,13 +1502,13 @@
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E39" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="13" t="s">
         <v>66</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1494,13 +1516,13 @@
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1508,13 +1530,13 @@
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E41" s="13" t="s">
-        <v>83</v>
-      </c>
       <c r="F41" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1522,13 +1544,13 @@
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E42" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1536,24 +1558,24 @@
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="E43" s="13" t="s">
-        <v>103</v>
-      </c>
       <c r="F43" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B45" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="15" t="s">
         <v>88</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>89</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
@@ -1564,13 +1586,13 @@
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E46" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="F46" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1578,13 +1600,13 @@
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
       <c r="D47" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1592,13 +1614,13 @@
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
       <c r="D48" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E48" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F48" s="15" t="s">
         <v>76</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1648,13 +1670,13 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1662,13 +1684,13 @@
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1676,13 +1698,13 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>